<commit_message>
test(sample): create new excel file with correct size
sizes of correct created excel file  and old sample  were not the same

#13
</commit_message>
<xml_diff>
--- a/__tests__/Fixtures/sample.xlsx
+++ b/__tests__/Fixtures/sample.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Question 1?" state="show" r:id="rId4"/>
-    <sheet sheetId="2" name="Question 2?" state="show" r:id="rId5"/>
+    <sheet sheetId="1" name="Question 1?" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Question 2?" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>

</xml_diff>

<commit_message>
test(export): fix bug test always passes true (#18)
</commit_message>
<xml_diff>
--- a/__tests__/Fixtures/sample.xlsx
+++ b/__tests__/Fixtures/sample.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Question 1?" state="show" r:id="rId4"/>
-    <sheet sheetId="2" name="Question 2?" state="show" r:id="rId5"/>
+    <sheet sheetId="1" name="Question 1?" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Question 2?" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>

</xml_diff>